<commit_message>
replace theme colors with standard colors in Excel template file
</commit_message>
<xml_diff>
--- a/template/xl-template.xlsx
+++ b/template/xl-template.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Personal Stuff\Coding\Personal\Musicnotes-Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Personal Stuff\Coding\Personal\Musicnotes-Reports\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C78432-6CB1-43C2-A1F0-B4FC27F30437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B683D73-C0C3-425C-BA35-9B134351438D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,12 +78,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -114,12 +108,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +134,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -148,34 +142,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -437,7 +431,7 @@
   <dimension ref="A2:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +439,7 @@
     <col min="1" max="1" width="47.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -455,7 +449,7 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -463,157 +457,157 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="5"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="5"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-      <c r="D10" s="8"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
-      <c r="D21" s="8"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="5"/>
-      <c r="D22" s="8"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
-      <c r="D23" s="8"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
-      <c r="D24" s="8"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
-      <c r="D25" s="8"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="5"/>
-      <c r="D26" s="8"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
-      <c r="D27" s="8"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="5"/>
-      <c r="D28" s="8"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
-      <c r="D29" s="8"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="5"/>
-      <c r="D30" s="8"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
-      <c r="D31" s="8"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="5"/>
-      <c r="D32" s="8"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
-      <c r="D33" s="8"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="5"/>
-      <c r="D34" s="8"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="8"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
-      <c r="D36" s="8"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
-      <c r="D37" s="8"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="5"/>
-      <c r="D38" s="8"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="6"/>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
-      <c r="D39" s="8"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
-      <c r="D40" s="8"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove border in template file
</commit_message>
<xml_diff>
--- a/template/xl-template.xlsx
+++ b/template/xl-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Personal Stuff\Coding\Personal\Musicnotes-Reports\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B683D73-C0C3-425C-BA35-9B134351438D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAC2F39-64E4-4366-BD44-2D43D24198A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,19 +82,10 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -103,17 +94,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D40"/>
+  <dimension ref="A2:D200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -436,178 +424,819 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="4"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="4"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="4"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="4"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="4"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="4"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="4"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="4"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="4"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="4"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="4"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="4"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="4"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="4"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="4"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="4"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="4"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="4"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="4"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="4"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="4"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+    </row>
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+    </row>
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+    </row>
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+    </row>
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+    </row>
+    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+    </row>
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+    </row>
+    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+    </row>
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+    </row>
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+    </row>
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+    </row>
+    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+    </row>
+    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+    </row>
+    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+    </row>
+    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+    </row>
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+    </row>
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+    </row>
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+    </row>
+    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+    </row>
+    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+    </row>
+    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+    </row>
+    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+    </row>
+    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+    </row>
+    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+    </row>
+    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+    </row>
+    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+    </row>
+    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+    </row>
+    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+    </row>
+    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+    </row>
+    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+    </row>
+    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+    </row>
+    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+    </row>
+    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+    </row>
+    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+    </row>
+    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+    </row>
+    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+    </row>
+    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+    </row>
+    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+    </row>
+    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+    </row>
+    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+    </row>
+    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+    </row>
+    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+    </row>
+    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
+    </row>
+    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+    </row>
+    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+    </row>
+    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+    </row>
+    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+    </row>
+    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+    </row>
+    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+    </row>
+    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+    </row>
+    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+    </row>
+    <row r="178" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+    </row>
+    <row r="179" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+    </row>
+    <row r="180" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
+    </row>
+    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
+    </row>
+    <row r="182" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C182" s="6"/>
+      <c r="D182" s="6"/>
+    </row>
+    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+    </row>
+    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C184" s="6"/>
+      <c r="D184" s="6"/>
+    </row>
+    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C185" s="6"/>
+      <c r="D185" s="6"/>
+    </row>
+    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+    </row>
+    <row r="187" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C187" s="6"/>
+      <c r="D187" s="6"/>
+    </row>
+    <row r="188" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C188" s="6"/>
+      <c r="D188" s="6"/>
+    </row>
+    <row r="189" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C189" s="6"/>
+      <c r="D189" s="6"/>
+    </row>
+    <row r="190" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C190" s="6"/>
+      <c r="D190" s="6"/>
+    </row>
+    <row r="191" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C191" s="6"/>
+      <c r="D191" s="6"/>
+    </row>
+    <row r="192" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C192" s="6"/>
+      <c r="D192" s="6"/>
+    </row>
+    <row r="193" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
+    </row>
+    <row r="194" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
+    </row>
+    <row r="195" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
+    </row>
+    <row r="196" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
+    </row>
+    <row r="197" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
+    </row>
+    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
+    </row>
+    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C199" s="6"/>
+      <c r="D199" s="6"/>
+    </row>
+    <row r="200" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C200" s="6"/>
+      <c r="D200" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>